<commit_message>
Add 2060 perturbation for ch4 and n20
</commit_message>
<xml_diff>
--- a/data/IWG_inputs/PAGE/Non-co2 perturbation data - 1 Mt.xlsx
+++ b/data/IWG_inputs/PAGE/Non-co2 perturbation data - 1 Mt.xlsx
@@ -1,30 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CGriffit\Documents\Climate Change\Non CO2 gases\Computer switch check (10-26-15)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bparthum\.julia\dev\MimiIWG\data\IWG_inputs\PAGE\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B500360-86E1-415D-A492-0F8D2E619F2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11580"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="21">
   <si>
     <t>Pertubation in the PAGE Excess Forcings vector due to a 1 Mt shock in CH4</t>
   </si>
@@ -82,11 +91,17 @@
   <si>
     <t>PAGE input: N2O Shock, 2050</t>
   </si>
+  <si>
+    <t>PAGE input: CH4 Shock, 2060</t>
+  </si>
+  <si>
+    <t>PAGE input: N2O Shock, 2060</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -426,21 +441,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AV27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AR4" sqref="AR4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -459,8 +474,11 @@
       <c r="AJ2" t="s">
         <v>6</v>
       </c>
+      <c r="AQ2" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -574,8 +592,26 @@
       <c r="AO3" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="AQ3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="AR3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AS3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AT3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AU3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AV3" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>2010</v>
       </c>
@@ -684,8 +720,26 @@
       <c r="AO4" s="5">
         <v>0</v>
       </c>
+      <c r="AQ4" s="5">
+        <v>2010</v>
+      </c>
+      <c r="AR4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AT4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AU4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV4" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>2020</v>
       </c>
@@ -794,8 +848,26 @@
       <c r="AO5" s="5">
         <v>0</v>
       </c>
+      <c r="AQ5" s="5">
+        <v>2020</v>
+      </c>
+      <c r="AR5" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS5" s="5">
+        <v>0</v>
+      </c>
+      <c r="AT5" s="5">
+        <v>0</v>
+      </c>
+      <c r="AU5" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV5" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>2030</v>
       </c>
@@ -904,8 +976,26 @@
       <c r="AO6" s="5">
         <v>0</v>
       </c>
+      <c r="AQ6" s="5">
+        <v>2030</v>
+      </c>
+      <c r="AR6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AT6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AU6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV6" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>2040</v>
       </c>
@@ -1014,8 +1104,26 @@
       <c r="AO7" s="5">
         <v>0</v>
       </c>
+      <c r="AQ7" s="5">
+        <v>2040</v>
+      </c>
+      <c r="AR7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AT7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AU7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV7" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>2050</v>
       </c>
@@ -1124,8 +1232,26 @@
       <c r="AO8" s="5">
         <v>1.1729308056250831E-4</v>
       </c>
+      <c r="AQ8" s="5">
+        <v>2050</v>
+      </c>
+      <c r="AR8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AT8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AU8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV8" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>2060</v>
       </c>
@@ -1234,8 +1360,26 @@
       <c r="AO9" s="5">
         <v>4.1096791080202919E-5</v>
       </c>
+      <c r="AQ9" s="5">
+        <v>2060</v>
+      </c>
+      <c r="AR9" s="5">
+        <v>7.1155643087639217E-5</v>
+      </c>
+      <c r="AS9" s="5">
+        <v>7.2944555823906132E-5</v>
+      </c>
+      <c r="AT9" s="5">
+        <v>7.508513712286557E-5</v>
+      </c>
+      <c r="AU9" s="5">
+        <v>7.6260473212275143E-5</v>
+      </c>
+      <c r="AV9" s="5">
+        <v>8.8229397874300955E-5</v>
+      </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>2080</v>
       </c>
@@ -1344,8 +1488,26 @@
       <c r="AO10" s="5">
         <v>7.2738827379847938E-6</v>
       </c>
+      <c r="AQ10" s="5">
+        <v>2080</v>
+      </c>
+      <c r="AR10" s="5">
+        <v>1.3418894915573354E-5</v>
+      </c>
+      <c r="AS10" s="5">
+        <v>1.4055531157619593E-5</v>
+      </c>
+      <c r="AT10" s="5">
+        <v>1.4544777158365107E-5</v>
+      </c>
+      <c r="AU10" s="5">
+        <v>1.4165668575349955E-5</v>
+      </c>
+      <c r="AV10" s="5">
+        <v>1.7364025824845309E-5</v>
+      </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>2100</v>
       </c>
@@ -1454,8 +1616,26 @@
       <c r="AO11" s="5">
         <v>3.0987515622915573E-7</v>
       </c>
+      <c r="AQ11" s="5">
+        <v>2100</v>
+      </c>
+      <c r="AR11" s="5">
+        <v>5.4923995536082519E-7</v>
+      </c>
+      <c r="AS11" s="5">
+        <v>5.9687074613901105E-7</v>
+      </c>
+      <c r="AT11" s="5">
+        <v>6.1714408356783323E-7</v>
+      </c>
+      <c r="AU11" s="5">
+        <v>5.7665128834427647E-7</v>
+      </c>
+      <c r="AV11" s="5">
+        <v>7.3930841433478277E-7</v>
+      </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>2200</v>
       </c>
@@ -1564,8 +1744,26 @@
       <c r="AO12" s="5">
         <v>5.1562142333594351E-11</v>
       </c>
+      <c r="AQ12" s="5">
+        <v>2200</v>
+      </c>
+      <c r="AR12" s="5">
+        <v>9.0322458401459472E-11</v>
+      </c>
+      <c r="AS12" s="5">
+        <v>9.9343540060914399E-11</v>
+      </c>
+      <c r="AT12" s="5">
+        <v>1.0258888849534743E-10</v>
+      </c>
+      <c r="AU12" s="5">
+        <v>9.4655263627174685E-11</v>
+      </c>
+      <c r="AV12" s="5">
+        <v>1.2292778128752957E-10</v>
+      </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>2300</v>
       </c>
@@ -1674,13 +1872,31 @@
       <c r="AO13" s="5">
         <v>7.2053474298172659E-14</v>
       </c>
+      <c r="AQ13" s="5">
+        <v>2300</v>
+      </c>
+      <c r="AR13" s="5">
+        <v>1.2501111257279263E-13</v>
+      </c>
+      <c r="AS13" s="5">
+        <v>1.3788969965844444E-13</v>
+      </c>
+      <c r="AT13" s="5">
+        <v>1.4233059175694507E-13</v>
+      </c>
+      <c r="AU13" s="5">
+        <v>1.3145040611561853E-13</v>
+      </c>
+      <c r="AV13" s="5">
+        <v>1.7053025658242404E-13</v>
+      </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -1699,8 +1915,11 @@
       <c r="AJ16" t="s">
         <v>18</v>
       </c>
+      <c r="AQ16" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
@@ -1814,8 +2033,26 @@
       <c r="AO17" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="AQ17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="AR17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AS17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AT17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AU17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AV17" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>2010</v>
       </c>
@@ -1924,8 +2161,26 @@
       <c r="AO18" s="5">
         <v>0</v>
       </c>
+      <c r="AQ18" s="5">
+        <v>2010</v>
+      </c>
+      <c r="AR18" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS18" s="5">
+        <v>0</v>
+      </c>
+      <c r="AT18" s="5">
+        <v>0</v>
+      </c>
+      <c r="AU18" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV18" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>2020</v>
       </c>
@@ -2034,8 +2289,26 @@
       <c r="AO19" s="5">
         <v>0</v>
       </c>
+      <c r="AQ19" s="5">
+        <v>2020</v>
+      </c>
+      <c r="AR19" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS19" s="5">
+        <v>0</v>
+      </c>
+      <c r="AT19" s="5">
+        <v>0</v>
+      </c>
+      <c r="AU19" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV19" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>2030</v>
       </c>
@@ -2144,8 +2417,26 @@
       <c r="AO20" s="5">
         <v>0</v>
       </c>
+      <c r="AQ20" s="5">
+        <v>2030</v>
+      </c>
+      <c r="AR20" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS20" s="5">
+        <v>0</v>
+      </c>
+      <c r="AT20" s="5">
+        <v>0</v>
+      </c>
+      <c r="AU20" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV20" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>2040</v>
       </c>
@@ -2254,8 +2545,26 @@
       <c r="AO21" s="5">
         <v>0</v>
       </c>
+      <c r="AQ21" s="5">
+        <v>2040</v>
+      </c>
+      <c r="AR21" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS21" s="5">
+        <v>0</v>
+      </c>
+      <c r="AT21" s="5">
+        <v>0</v>
+      </c>
+      <c r="AU21" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV21" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>2050</v>
       </c>
@@ -2364,8 +2673,26 @@
       <c r="AO22" s="5">
         <v>3.4205293054798136E-4</v>
       </c>
+      <c r="AQ22" s="5">
+        <v>2050</v>
+      </c>
+      <c r="AR22" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS22" s="5">
+        <v>0</v>
+      </c>
+      <c r="AT22" s="5">
+        <v>0</v>
+      </c>
+      <c r="AU22" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV22" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>2060</v>
       </c>
@@ -2474,8 +2801,26 @@
       <c r="AO23" s="5">
         <v>3.3083344047559751E-4</v>
       </c>
+      <c r="AQ23" s="5">
+        <v>2060</v>
+      </c>
+      <c r="AR23" s="5">
+        <v>3.4756994042368374E-4</v>
+      </c>
+      <c r="AS23" s="5">
+        <v>3.2965924978970161E-4</v>
+      </c>
+      <c r="AT23" s="5">
+        <v>3.2867020376360357E-4</v>
+      </c>
+      <c r="AU23" s="5">
+        <v>3.3633103433914903E-4</v>
+      </c>
+      <c r="AV23" s="5">
+        <v>3.4154397442547058E-4</v>
+      </c>
     </row>
-    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>2080</v>
       </c>
@@ -2584,8 +2929,26 @@
       <c r="AO24" s="5">
         <v>2.7424171966061451E-4</v>
       </c>
+      <c r="AQ24" s="5">
+        <v>2080</v>
+      </c>
+      <c r="AR24" s="5">
+        <v>3.0442179878799878E-4</v>
+      </c>
+      <c r="AS24" s="5">
+        <v>2.8776869401197781E-4</v>
+      </c>
+      <c r="AT24" s="5">
+        <v>2.8413111429783646E-4</v>
+      </c>
+      <c r="AU24" s="5">
+        <v>2.9299055979585542E-4</v>
+      </c>
+      <c r="AV24" s="5">
+        <v>2.9949878678081908E-4</v>
+      </c>
     </row>
-    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>2100</v>
       </c>
@@ -2694,8 +3057,26 @@
       <c r="AO25" s="5">
         <v>1.6594585305878095E-4</v>
       </c>
+      <c r="AQ25" s="5">
+        <v>2100</v>
+      </c>
+      <c r="AR25" s="5">
+        <v>1.8109292692546631E-4</v>
+      </c>
+      <c r="AS25" s="5">
+        <v>1.7303499667413347E-4</v>
+      </c>
+      <c r="AT25" s="5">
+        <v>1.6545806484028424E-4</v>
+      </c>
+      <c r="AU25" s="5">
+        <v>1.7257920543678807E-4</v>
+      </c>
+      <c r="AV25" s="5">
+        <v>1.7937031897590828E-4</v>
+      </c>
     </row>
-    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>2200</v>
       </c>
@@ -2804,8 +3185,26 @@
       <c r="AO26" s="5">
         <v>6.8759670866003764E-5</v>
       </c>
+      <c r="AQ26" s="5">
+        <v>2200</v>
+      </c>
+      <c r="AR26" s="5">
+        <v>7.3388024830025605E-5</v>
+      </c>
+      <c r="AS26" s="5">
+        <v>7.101522016244311E-5</v>
+      </c>
+      <c r="AT26" s="5">
+        <v>6.5696502927544692E-5</v>
+      </c>
+      <c r="AU26" s="5">
+        <v>6.9260370142663059E-5</v>
+      </c>
+      <c r="AV26" s="5">
+        <v>7.3215175532643782E-5</v>
+      </c>
     </row>
-    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>2300</v>
       </c>
@@ -2913,6 +3312,24 @@
       </c>
       <c r="AO27" s="5">
         <v>4.2672421670941763E-5</v>
+      </c>
+      <c r="AQ27" s="5">
+        <v>2300</v>
+      </c>
+      <c r="AR27" s="5">
+        <v>4.5256296990203726E-5</v>
+      </c>
+      <c r="AS27" s="5">
+        <v>4.3949774506890638E-5</v>
+      </c>
+      <c r="AT27" s="5">
+        <v>4.0290512913099263E-5</v>
+      </c>
+      <c r="AU27" s="5">
+        <v>4.2597198992688767E-5</v>
+      </c>
+      <c r="AV27" s="5">
+        <v>4.5240913177369002E-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add 2060 perturbation for ch4 and n2o
</commit_message>
<xml_diff>
--- a/data/IWG_inputs/PAGE/Non-co2 perturbation data - 1 Mt.xlsx
+++ b/data/IWG_inputs/PAGE/Non-co2 perturbation data - 1 Mt.xlsx
@@ -1,30 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CGriffit\Documents\Climate Change\Non CO2 gases\Computer switch check (10-26-15)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bparthum\.julia\dev\MimiIWG\data\IWG_inputs\PAGE\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B500360-86E1-415D-A492-0F8D2E619F2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11580"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="21">
   <si>
     <t>Pertubation in the PAGE Excess Forcings vector due to a 1 Mt shock in CH4</t>
   </si>
@@ -82,11 +91,17 @@
   <si>
     <t>PAGE input: N2O Shock, 2050</t>
   </si>
+  <si>
+    <t>PAGE input: CH4 Shock, 2060</t>
+  </si>
+  <si>
+    <t>PAGE input: N2O Shock, 2060</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -426,21 +441,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AV27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AR4" sqref="AR4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -459,8 +474,11 @@
       <c r="AJ2" t="s">
         <v>6</v>
       </c>
+      <c r="AQ2" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -574,8 +592,26 @@
       <c r="AO3" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="AQ3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="AR3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AS3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AT3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AU3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AV3" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>2010</v>
       </c>
@@ -684,8 +720,26 @@
       <c r="AO4" s="5">
         <v>0</v>
       </c>
+      <c r="AQ4" s="5">
+        <v>2010</v>
+      </c>
+      <c r="AR4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AT4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AU4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV4" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>2020</v>
       </c>
@@ -794,8 +848,26 @@
       <c r="AO5" s="5">
         <v>0</v>
       </c>
+      <c r="AQ5" s="5">
+        <v>2020</v>
+      </c>
+      <c r="AR5" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS5" s="5">
+        <v>0</v>
+      </c>
+      <c r="AT5" s="5">
+        <v>0</v>
+      </c>
+      <c r="AU5" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV5" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>2030</v>
       </c>
@@ -904,8 +976,26 @@
       <c r="AO6" s="5">
         <v>0</v>
       </c>
+      <c r="AQ6" s="5">
+        <v>2030</v>
+      </c>
+      <c r="AR6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AT6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AU6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV6" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>2040</v>
       </c>
@@ -1014,8 +1104,26 @@
       <c r="AO7" s="5">
         <v>0</v>
       </c>
+      <c r="AQ7" s="5">
+        <v>2040</v>
+      </c>
+      <c r="AR7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AT7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AU7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV7" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>2050</v>
       </c>
@@ -1124,8 +1232,26 @@
       <c r="AO8" s="5">
         <v>1.1729308056250831E-4</v>
       </c>
+      <c r="AQ8" s="5">
+        <v>2050</v>
+      </c>
+      <c r="AR8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AT8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AU8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV8" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>2060</v>
       </c>
@@ -1234,8 +1360,26 @@
       <c r="AO9" s="5">
         <v>4.1096791080202919E-5</v>
       </c>
+      <c r="AQ9" s="5">
+        <v>2060</v>
+      </c>
+      <c r="AR9" s="5">
+        <v>7.1155643087639217E-5</v>
+      </c>
+      <c r="AS9" s="5">
+        <v>7.2944555823906132E-5</v>
+      </c>
+      <c r="AT9" s="5">
+        <v>7.508513712286557E-5</v>
+      </c>
+      <c r="AU9" s="5">
+        <v>7.6260473212275143E-5</v>
+      </c>
+      <c r="AV9" s="5">
+        <v>8.8229397874300955E-5</v>
+      </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>2080</v>
       </c>
@@ -1344,8 +1488,26 @@
       <c r="AO10" s="5">
         <v>7.2738827379847938E-6</v>
       </c>
+      <c r="AQ10" s="5">
+        <v>2080</v>
+      </c>
+      <c r="AR10" s="5">
+        <v>1.3418894915573354E-5</v>
+      </c>
+      <c r="AS10" s="5">
+        <v>1.4055531157619593E-5</v>
+      </c>
+      <c r="AT10" s="5">
+        <v>1.4544777158365107E-5</v>
+      </c>
+      <c r="AU10" s="5">
+        <v>1.4165668575349955E-5</v>
+      </c>
+      <c r="AV10" s="5">
+        <v>1.7364025824845309E-5</v>
+      </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>2100</v>
       </c>
@@ -1454,8 +1616,26 @@
       <c r="AO11" s="5">
         <v>3.0987515622915573E-7</v>
       </c>
+      <c r="AQ11" s="5">
+        <v>2100</v>
+      </c>
+      <c r="AR11" s="5">
+        <v>5.4923995536082519E-7</v>
+      </c>
+      <c r="AS11" s="5">
+        <v>5.9687074613901105E-7</v>
+      </c>
+      <c r="AT11" s="5">
+        <v>6.1714408356783323E-7</v>
+      </c>
+      <c r="AU11" s="5">
+        <v>5.7665128834427647E-7</v>
+      </c>
+      <c r="AV11" s="5">
+        <v>7.3930841433478277E-7</v>
+      </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>2200</v>
       </c>
@@ -1564,8 +1744,26 @@
       <c r="AO12" s="5">
         <v>5.1562142333594351E-11</v>
       </c>
+      <c r="AQ12" s="5">
+        <v>2200</v>
+      </c>
+      <c r="AR12" s="5">
+        <v>9.0322458401459472E-11</v>
+      </c>
+      <c r="AS12" s="5">
+        <v>9.9343540060914399E-11</v>
+      </c>
+      <c r="AT12" s="5">
+        <v>1.0258888849534743E-10</v>
+      </c>
+      <c r="AU12" s="5">
+        <v>9.4655263627174685E-11</v>
+      </c>
+      <c r="AV12" s="5">
+        <v>1.2292778128752957E-10</v>
+      </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>2300</v>
       </c>
@@ -1674,13 +1872,31 @@
       <c r="AO13" s="5">
         <v>7.2053474298172659E-14</v>
       </c>
+      <c r="AQ13" s="5">
+        <v>2300</v>
+      </c>
+      <c r="AR13" s="5">
+        <v>1.2501111257279263E-13</v>
+      </c>
+      <c r="AS13" s="5">
+        <v>1.3788969965844444E-13</v>
+      </c>
+      <c r="AT13" s="5">
+        <v>1.4233059175694507E-13</v>
+      </c>
+      <c r="AU13" s="5">
+        <v>1.3145040611561853E-13</v>
+      </c>
+      <c r="AV13" s="5">
+        <v>1.7053025658242404E-13</v>
+      </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -1699,8 +1915,11 @@
       <c r="AJ16" t="s">
         <v>18</v>
       </c>
+      <c r="AQ16" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
@@ -1814,8 +2033,26 @@
       <c r="AO17" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="AQ17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="AR17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AS17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AT17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AU17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AV17" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>2010</v>
       </c>
@@ -1924,8 +2161,26 @@
       <c r="AO18" s="5">
         <v>0</v>
       </c>
+      <c r="AQ18" s="5">
+        <v>2010</v>
+      </c>
+      <c r="AR18" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS18" s="5">
+        <v>0</v>
+      </c>
+      <c r="AT18" s="5">
+        <v>0</v>
+      </c>
+      <c r="AU18" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV18" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>2020</v>
       </c>
@@ -2034,8 +2289,26 @@
       <c r="AO19" s="5">
         <v>0</v>
       </c>
+      <c r="AQ19" s="5">
+        <v>2020</v>
+      </c>
+      <c r="AR19" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS19" s="5">
+        <v>0</v>
+      </c>
+      <c r="AT19" s="5">
+        <v>0</v>
+      </c>
+      <c r="AU19" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV19" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>2030</v>
       </c>
@@ -2144,8 +2417,26 @@
       <c r="AO20" s="5">
         <v>0</v>
       </c>
+      <c r="AQ20" s="5">
+        <v>2030</v>
+      </c>
+      <c r="AR20" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS20" s="5">
+        <v>0</v>
+      </c>
+      <c r="AT20" s="5">
+        <v>0</v>
+      </c>
+      <c r="AU20" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV20" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>2040</v>
       </c>
@@ -2254,8 +2545,26 @@
       <c r="AO21" s="5">
         <v>0</v>
       </c>
+      <c r="AQ21" s="5">
+        <v>2040</v>
+      </c>
+      <c r="AR21" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS21" s="5">
+        <v>0</v>
+      </c>
+      <c r="AT21" s="5">
+        <v>0</v>
+      </c>
+      <c r="AU21" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV21" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>2050</v>
       </c>
@@ -2364,8 +2673,26 @@
       <c r="AO22" s="5">
         <v>3.4205293054798136E-4</v>
       </c>
+      <c r="AQ22" s="5">
+        <v>2050</v>
+      </c>
+      <c r="AR22" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS22" s="5">
+        <v>0</v>
+      </c>
+      <c r="AT22" s="5">
+        <v>0</v>
+      </c>
+      <c r="AU22" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV22" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>2060</v>
       </c>
@@ -2474,8 +2801,26 @@
       <c r="AO23" s="5">
         <v>3.3083344047559751E-4</v>
       </c>
+      <c r="AQ23" s="5">
+        <v>2060</v>
+      </c>
+      <c r="AR23" s="5">
+        <v>3.4756994042368374E-4</v>
+      </c>
+      <c r="AS23" s="5">
+        <v>3.2965924978970161E-4</v>
+      </c>
+      <c r="AT23" s="5">
+        <v>3.2867020376360357E-4</v>
+      </c>
+      <c r="AU23" s="5">
+        <v>3.3633103433914903E-4</v>
+      </c>
+      <c r="AV23" s="5">
+        <v>3.4154397442547058E-4</v>
+      </c>
     </row>
-    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>2080</v>
       </c>
@@ -2584,8 +2929,26 @@
       <c r="AO24" s="5">
         <v>2.7424171966061451E-4</v>
       </c>
+      <c r="AQ24" s="5">
+        <v>2080</v>
+      </c>
+      <c r="AR24" s="5">
+        <v>3.0442179878799878E-4</v>
+      </c>
+      <c r="AS24" s="5">
+        <v>2.8776869401197781E-4</v>
+      </c>
+      <c r="AT24" s="5">
+        <v>2.8413111429783646E-4</v>
+      </c>
+      <c r="AU24" s="5">
+        <v>2.9299055979585542E-4</v>
+      </c>
+      <c r="AV24" s="5">
+        <v>2.9949878678081908E-4</v>
+      </c>
     </row>
-    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>2100</v>
       </c>
@@ -2694,8 +3057,26 @@
       <c r="AO25" s="5">
         <v>1.6594585305878095E-4</v>
       </c>
+      <c r="AQ25" s="5">
+        <v>2100</v>
+      </c>
+      <c r="AR25" s="5">
+        <v>1.8109292692546631E-4</v>
+      </c>
+      <c r="AS25" s="5">
+        <v>1.7303499667413347E-4</v>
+      </c>
+      <c r="AT25" s="5">
+        <v>1.6545806484028424E-4</v>
+      </c>
+      <c r="AU25" s="5">
+        <v>1.7257920543678807E-4</v>
+      </c>
+      <c r="AV25" s="5">
+        <v>1.7937031897590828E-4</v>
+      </c>
     </row>
-    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>2200</v>
       </c>
@@ -2804,8 +3185,26 @@
       <c r="AO26" s="5">
         <v>6.8759670866003764E-5</v>
       </c>
+      <c r="AQ26" s="5">
+        <v>2200</v>
+      </c>
+      <c r="AR26" s="5">
+        <v>7.3388024830025605E-5</v>
+      </c>
+      <c r="AS26" s="5">
+        <v>7.101522016244311E-5</v>
+      </c>
+      <c r="AT26" s="5">
+        <v>6.5696502927544692E-5</v>
+      </c>
+      <c r="AU26" s="5">
+        <v>6.9260370142663059E-5</v>
+      </c>
+      <c r="AV26" s="5">
+        <v>7.3215175532643782E-5</v>
+      </c>
     </row>
-    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>2300</v>
       </c>
@@ -2913,6 +3312,24 @@
       </c>
       <c r="AO27" s="5">
         <v>4.2672421670941763E-5</v>
+      </c>
+      <c r="AQ27" s="5">
+        <v>2300</v>
+      </c>
+      <c r="AR27" s="5">
+        <v>4.5256296990203726E-5</v>
+      </c>
+      <c r="AS27" s="5">
+        <v>4.3949774506890638E-5</v>
+      </c>
+      <c r="AT27" s="5">
+        <v>4.0290512913099263E-5</v>
+      </c>
+      <c r="AU27" s="5">
+        <v>4.2597198992688767E-5</v>
+      </c>
+      <c r="AV27" s="5">
+        <v>4.5240913177369002E-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Added 2060 perturbation for ch4 and n2o"
</commit_message>
<xml_diff>
--- a/data/IWG_inputs/PAGE/Non-co2 perturbation data - 1 Mt.xlsx
+++ b/data/IWG_inputs/PAGE/Non-co2 perturbation data - 1 Mt.xlsx
@@ -1,39 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bparthum\.julia\dev\MimiIWG\data\IWG_inputs\PAGE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CGriffit\Documents\Climate Change\Non CO2 gases\Computer switch check (10-26-15)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B500360-86E1-415D-A492-0F8D2E619F2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11580"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="19">
   <si>
     <t>Pertubation in the PAGE Excess Forcings vector due to a 1 Mt shock in CH4</t>
   </si>
@@ -91,17 +82,11 @@
   <si>
     <t>PAGE input: N2O Shock, 2050</t>
   </si>
-  <si>
-    <t>PAGE input: CH4 Shock, 2060</t>
-  </si>
-  <si>
-    <t>PAGE input: N2O Shock, 2060</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -441,21 +426,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AV27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AO27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AR4" sqref="AR4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -474,11 +459,8 @@
       <c r="AJ2" t="s">
         <v>6</v>
       </c>
-      <c r="AQ2" t="s">
-        <v>19</v>
-      </c>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -592,26 +574,8 @@
       <c r="AO3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="AQ3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="AR3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AS3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="AT3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="AU3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="AV3" s="4" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2010</v>
       </c>
@@ -720,26 +684,8 @@
       <c r="AO4" s="5">
         <v>0</v>
       </c>
-      <c r="AQ4" s="5">
-        <v>2010</v>
-      </c>
-      <c r="AR4" s="5">
-        <v>0</v>
-      </c>
-      <c r="AS4" s="5">
-        <v>0</v>
-      </c>
-      <c r="AT4" s="5">
-        <v>0</v>
-      </c>
-      <c r="AU4" s="5">
-        <v>0</v>
-      </c>
-      <c r="AV4" s="5">
-        <v>0</v>
-      </c>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2020</v>
       </c>
@@ -848,26 +794,8 @@
       <c r="AO5" s="5">
         <v>0</v>
       </c>
-      <c r="AQ5" s="5">
-        <v>2020</v>
-      </c>
-      <c r="AR5" s="5">
-        <v>0</v>
-      </c>
-      <c r="AS5" s="5">
-        <v>0</v>
-      </c>
-      <c r="AT5" s="5">
-        <v>0</v>
-      </c>
-      <c r="AU5" s="5">
-        <v>0</v>
-      </c>
-      <c r="AV5" s="5">
-        <v>0</v>
-      </c>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>2030</v>
       </c>
@@ -976,26 +904,8 @@
       <c r="AO6" s="5">
         <v>0</v>
       </c>
-      <c r="AQ6" s="5">
-        <v>2030</v>
-      </c>
-      <c r="AR6" s="5">
-        <v>0</v>
-      </c>
-      <c r="AS6" s="5">
-        <v>0</v>
-      </c>
-      <c r="AT6" s="5">
-        <v>0</v>
-      </c>
-      <c r="AU6" s="5">
-        <v>0</v>
-      </c>
-      <c r="AV6" s="5">
-        <v>0</v>
-      </c>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>2040</v>
       </c>
@@ -1104,26 +1014,8 @@
       <c r="AO7" s="5">
         <v>0</v>
       </c>
-      <c r="AQ7" s="5">
-        <v>2040</v>
-      </c>
-      <c r="AR7" s="5">
-        <v>0</v>
-      </c>
-      <c r="AS7" s="5">
-        <v>0</v>
-      </c>
-      <c r="AT7" s="5">
-        <v>0</v>
-      </c>
-      <c r="AU7" s="5">
-        <v>0</v>
-      </c>
-      <c r="AV7" s="5">
-        <v>0</v>
-      </c>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>2050</v>
       </c>
@@ -1232,26 +1124,8 @@
       <c r="AO8" s="5">
         <v>1.1729308056250831E-4</v>
       </c>
-      <c r="AQ8" s="5">
-        <v>2050</v>
-      </c>
-      <c r="AR8" s="5">
-        <v>0</v>
-      </c>
-      <c r="AS8" s="5">
-        <v>0</v>
-      </c>
-      <c r="AT8" s="5">
-        <v>0</v>
-      </c>
-      <c r="AU8" s="5">
-        <v>0</v>
-      </c>
-      <c r="AV8" s="5">
-        <v>0</v>
-      </c>
     </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>2060</v>
       </c>
@@ -1360,26 +1234,8 @@
       <c r="AO9" s="5">
         <v>4.1096791080202919E-5</v>
       </c>
-      <c r="AQ9" s="5">
-        <v>2060</v>
-      </c>
-      <c r="AR9" s="5">
-        <v>7.1155643087639217E-5</v>
-      </c>
-      <c r="AS9" s="5">
-        <v>7.2944555823906132E-5</v>
-      </c>
-      <c r="AT9" s="5">
-        <v>7.508513712286557E-5</v>
-      </c>
-      <c r="AU9" s="5">
-        <v>7.6260473212275143E-5</v>
-      </c>
-      <c r="AV9" s="5">
-        <v>8.8229397874300955E-5</v>
-      </c>
     </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>2080</v>
       </c>
@@ -1488,26 +1344,8 @@
       <c r="AO10" s="5">
         <v>7.2738827379847938E-6</v>
       </c>
-      <c r="AQ10" s="5">
-        <v>2080</v>
-      </c>
-      <c r="AR10" s="5">
-        <v>1.3418894915573354E-5</v>
-      </c>
-      <c r="AS10" s="5">
-        <v>1.4055531157619593E-5</v>
-      </c>
-      <c r="AT10" s="5">
-        <v>1.4544777158365107E-5</v>
-      </c>
-      <c r="AU10" s="5">
-        <v>1.4165668575349955E-5</v>
-      </c>
-      <c r="AV10" s="5">
-        <v>1.7364025824845309E-5</v>
-      </c>
     </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>2100</v>
       </c>
@@ -1616,26 +1454,8 @@
       <c r="AO11" s="5">
         <v>3.0987515622915573E-7</v>
       </c>
-      <c r="AQ11" s="5">
-        <v>2100</v>
-      </c>
-      <c r="AR11" s="5">
-        <v>5.4923995536082519E-7</v>
-      </c>
-      <c r="AS11" s="5">
-        <v>5.9687074613901105E-7</v>
-      </c>
-      <c r="AT11" s="5">
-        <v>6.1714408356783323E-7</v>
-      </c>
-      <c r="AU11" s="5">
-        <v>5.7665128834427647E-7</v>
-      </c>
-      <c r="AV11" s="5">
-        <v>7.3930841433478277E-7</v>
-      </c>
     </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>2200</v>
       </c>
@@ -1744,26 +1564,8 @@
       <c r="AO12" s="5">
         <v>5.1562142333594351E-11</v>
       </c>
-      <c r="AQ12" s="5">
-        <v>2200</v>
-      </c>
-      <c r="AR12" s="5">
-        <v>9.0322458401459472E-11</v>
-      </c>
-      <c r="AS12" s="5">
-        <v>9.9343540060914399E-11</v>
-      </c>
-      <c r="AT12" s="5">
-        <v>1.0258888849534743E-10</v>
-      </c>
-      <c r="AU12" s="5">
-        <v>9.4655263627174685E-11</v>
-      </c>
-      <c r="AV12" s="5">
-        <v>1.2292778128752957E-10</v>
-      </c>
     </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>2300</v>
       </c>
@@ -1872,31 +1674,13 @@
       <c r="AO13" s="5">
         <v>7.2053474298172659E-14</v>
       </c>
-      <c r="AQ13" s="5">
-        <v>2300</v>
-      </c>
-      <c r="AR13" s="5">
-        <v>1.2501111257279263E-13</v>
-      </c>
-      <c r="AS13" s="5">
-        <v>1.3788969965844444E-13</v>
-      </c>
-      <c r="AT13" s="5">
-        <v>1.4233059175694507E-13</v>
-      </c>
-      <c r="AU13" s="5">
-        <v>1.3145040611561853E-13</v>
-      </c>
-      <c r="AV13" s="5">
-        <v>1.7053025658242404E-13</v>
-      </c>
     </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -1915,11 +1699,8 @@
       <c r="AJ16" t="s">
         <v>18</v>
       </c>
-      <c r="AQ16" t="s">
-        <v>20</v>
-      </c>
     </row>
-    <row r="17" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
@@ -2033,26 +1814,8 @@
       <c r="AO17" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="AQ17" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="AR17" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AS17" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="AT17" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="AU17" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="AV17" s="4" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="18" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>2010</v>
       </c>
@@ -2161,26 +1924,8 @@
       <c r="AO18" s="5">
         <v>0</v>
       </c>
-      <c r="AQ18" s="5">
-        <v>2010</v>
-      </c>
-      <c r="AR18" s="5">
-        <v>0</v>
-      </c>
-      <c r="AS18" s="5">
-        <v>0</v>
-      </c>
-      <c r="AT18" s="5">
-        <v>0</v>
-      </c>
-      <c r="AU18" s="5">
-        <v>0</v>
-      </c>
-      <c r="AV18" s="5">
-        <v>0</v>
-      </c>
     </row>
-    <row r="19" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>2020</v>
       </c>
@@ -2289,26 +2034,8 @@
       <c r="AO19" s="5">
         <v>0</v>
       </c>
-      <c r="AQ19" s="5">
-        <v>2020</v>
-      </c>
-      <c r="AR19" s="5">
-        <v>0</v>
-      </c>
-      <c r="AS19" s="5">
-        <v>0</v>
-      </c>
-      <c r="AT19" s="5">
-        <v>0</v>
-      </c>
-      <c r="AU19" s="5">
-        <v>0</v>
-      </c>
-      <c r="AV19" s="5">
-        <v>0</v>
-      </c>
     </row>
-    <row r="20" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>2030</v>
       </c>
@@ -2417,26 +2144,8 @@
       <c r="AO20" s="5">
         <v>0</v>
       </c>
-      <c r="AQ20" s="5">
-        <v>2030</v>
-      </c>
-      <c r="AR20" s="5">
-        <v>0</v>
-      </c>
-      <c r="AS20" s="5">
-        <v>0</v>
-      </c>
-      <c r="AT20" s="5">
-        <v>0</v>
-      </c>
-      <c r="AU20" s="5">
-        <v>0</v>
-      </c>
-      <c r="AV20" s="5">
-        <v>0</v>
-      </c>
     </row>
-    <row r="21" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>2040</v>
       </c>
@@ -2545,26 +2254,8 @@
       <c r="AO21" s="5">
         <v>0</v>
       </c>
-      <c r="AQ21" s="5">
-        <v>2040</v>
-      </c>
-      <c r="AR21" s="5">
-        <v>0</v>
-      </c>
-      <c r="AS21" s="5">
-        <v>0</v>
-      </c>
-      <c r="AT21" s="5">
-        <v>0</v>
-      </c>
-      <c r="AU21" s="5">
-        <v>0</v>
-      </c>
-      <c r="AV21" s="5">
-        <v>0</v>
-      </c>
     </row>
-    <row r="22" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>2050</v>
       </c>
@@ -2673,26 +2364,8 @@
       <c r="AO22" s="5">
         <v>3.4205293054798136E-4</v>
       </c>
-      <c r="AQ22" s="5">
-        <v>2050</v>
-      </c>
-      <c r="AR22" s="5">
-        <v>0</v>
-      </c>
-      <c r="AS22" s="5">
-        <v>0</v>
-      </c>
-      <c r="AT22" s="5">
-        <v>0</v>
-      </c>
-      <c r="AU22" s="5">
-        <v>0</v>
-      </c>
-      <c r="AV22" s="5">
-        <v>0</v>
-      </c>
     </row>
-    <row r="23" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>2060</v>
       </c>
@@ -2801,26 +2474,8 @@
       <c r="AO23" s="5">
         <v>3.3083344047559751E-4</v>
       </c>
-      <c r="AQ23" s="5">
-        <v>2060</v>
-      </c>
-      <c r="AR23" s="5">
-        <v>3.4756994042368374E-4</v>
-      </c>
-      <c r="AS23" s="5">
-        <v>3.2965924978970161E-4</v>
-      </c>
-      <c r="AT23" s="5">
-        <v>3.2867020376360357E-4</v>
-      </c>
-      <c r="AU23" s="5">
-        <v>3.3633103433914903E-4</v>
-      </c>
-      <c r="AV23" s="5">
-        <v>3.4154397442547058E-4</v>
-      </c>
     </row>
-    <row r="24" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>2080</v>
       </c>
@@ -2929,26 +2584,8 @@
       <c r="AO24" s="5">
         <v>2.7424171966061451E-4</v>
       </c>
-      <c r="AQ24" s="5">
-        <v>2080</v>
-      </c>
-      <c r="AR24" s="5">
-        <v>3.0442179878799878E-4</v>
-      </c>
-      <c r="AS24" s="5">
-        <v>2.8776869401197781E-4</v>
-      </c>
-      <c r="AT24" s="5">
-        <v>2.8413111429783646E-4</v>
-      </c>
-      <c r="AU24" s="5">
-        <v>2.9299055979585542E-4</v>
-      </c>
-      <c r="AV24" s="5">
-        <v>2.9949878678081908E-4</v>
-      </c>
     </row>
-    <row r="25" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>2100</v>
       </c>
@@ -3057,26 +2694,8 @@
       <c r="AO25" s="5">
         <v>1.6594585305878095E-4</v>
       </c>
-      <c r="AQ25" s="5">
-        <v>2100</v>
-      </c>
-      <c r="AR25" s="5">
-        <v>1.8109292692546631E-4</v>
-      </c>
-      <c r="AS25" s="5">
-        <v>1.7303499667413347E-4</v>
-      </c>
-      <c r="AT25" s="5">
-        <v>1.6545806484028424E-4</v>
-      </c>
-      <c r="AU25" s="5">
-        <v>1.7257920543678807E-4</v>
-      </c>
-      <c r="AV25" s="5">
-        <v>1.7937031897590828E-4</v>
-      </c>
     </row>
-    <row r="26" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>2200</v>
       </c>
@@ -3185,26 +2804,8 @@
       <c r="AO26" s="5">
         <v>6.8759670866003764E-5</v>
       </c>
-      <c r="AQ26" s="5">
-        <v>2200</v>
-      </c>
-      <c r="AR26" s="5">
-        <v>7.3388024830025605E-5</v>
-      </c>
-      <c r="AS26" s="5">
-        <v>7.101522016244311E-5</v>
-      </c>
-      <c r="AT26" s="5">
-        <v>6.5696502927544692E-5</v>
-      </c>
-      <c r="AU26" s="5">
-        <v>6.9260370142663059E-5</v>
-      </c>
-      <c r="AV26" s="5">
-        <v>7.3215175532643782E-5</v>
-      </c>
     </row>
-    <row r="27" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>2300</v>
       </c>
@@ -3312,24 +2913,6 @@
       </c>
       <c r="AO27" s="5">
         <v>4.2672421670941763E-5</v>
-      </c>
-      <c r="AQ27" s="5">
-        <v>2300</v>
-      </c>
-      <c r="AR27" s="5">
-        <v>4.5256296990203726E-5</v>
-      </c>
-      <c r="AS27" s="5">
-        <v>4.3949774506890638E-5</v>
-      </c>
-      <c r="AT27" s="5">
-        <v>4.0290512913099263E-5</v>
-      </c>
-      <c r="AU27" s="5">
-        <v>4.2597198992688767E-5</v>
-      </c>
-      <c r="AV27" s="5">
-        <v>4.5240913177369002E-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add option for 2080 PAGE perturbatoin
</commit_message>
<xml_diff>
--- a/data/IWG_inputs/PAGE/Non-co2 perturbation data - 1 Mt.xlsx
+++ b/data/IWG_inputs/PAGE/Non-co2 perturbation data - 1 Mt.xlsx
@@ -1,39 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bparthum\.julia\dev\MimiIWG\data\IWG_inputs\PAGE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lisarennels/.julia/dev/MimiIWG/data/IWG_inputs/PAGE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B500360-86E1-415D-A492-0F8D2E619F2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9501AAC-96CF-3F4E-8392-9A617DDDAF53}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3720" yWindow="1200" windowWidth="27620" windowHeight="18160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="23">
   <si>
     <t>Pertubation in the PAGE Excess Forcings vector due to a 1 Mt shock in CH4</t>
   </si>
@@ -96,6 +88,12 @@
   </si>
   <si>
     <t>PAGE input: N2O Shock, 2060</t>
+  </si>
+  <si>
+    <t>PAGE input: CH4 Shock, 2080</t>
+  </si>
+  <si>
+    <t>PAGE input: N2O Shock, 2080</t>
   </si>
 </sst>
 </file>
@@ -442,20 +440,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AV27"/>
+  <dimension ref="A1:BC27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AR4" sqref="AR4"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
+      <selection activeCell="AQ13" sqref="AQ13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -477,8 +475,11 @@
       <c r="AQ2" t="s">
         <v>19</v>
       </c>
+      <c r="AX2" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -610,8 +611,26 @@
       <c r="AV3" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="AX3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="AY3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AZ3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="BA3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="BB3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="BC3" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>2010</v>
       </c>
@@ -738,8 +757,26 @@
       <c r="AV4" s="5">
         <v>0</v>
       </c>
+      <c r="AX4" s="5">
+        <v>2010</v>
+      </c>
+      <c r="AY4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ4" s="5">
+        <v>0</v>
+      </c>
+      <c r="BA4" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB4" s="5">
+        <v>0</v>
+      </c>
+      <c r="BC4" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>2020</v>
       </c>
@@ -866,8 +903,26 @@
       <c r="AV5" s="5">
         <v>0</v>
       </c>
+      <c r="AX5" s="5">
+        <v>2020</v>
+      </c>
+      <c r="AY5" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ5" s="5">
+        <v>0</v>
+      </c>
+      <c r="BA5" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB5" s="5">
+        <v>0</v>
+      </c>
+      <c r="BC5" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>2030</v>
       </c>
@@ -994,8 +1049,26 @@
       <c r="AV6" s="5">
         <v>0</v>
       </c>
+      <c r="AX6" s="5">
+        <v>2030</v>
+      </c>
+      <c r="AY6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ6" s="5">
+        <v>0</v>
+      </c>
+      <c r="BA6" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB6" s="5">
+        <v>0</v>
+      </c>
+      <c r="BC6" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>2040</v>
       </c>
@@ -1122,8 +1195,26 @@
       <c r="AV7" s="5">
         <v>0</v>
       </c>
+      <c r="AX7" s="5">
+        <v>2040</v>
+      </c>
+      <c r="AY7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ7" s="5">
+        <v>0</v>
+      </c>
+      <c r="BA7" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB7" s="5">
+        <v>0</v>
+      </c>
+      <c r="BC7" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>2050</v>
       </c>
@@ -1250,8 +1341,26 @@
       <c r="AV8" s="5">
         <v>0</v>
       </c>
+      <c r="AX8" s="5">
+        <v>2050</v>
+      </c>
+      <c r="AY8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ8" s="5">
+        <v>0</v>
+      </c>
+      <c r="BA8" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB8" s="5">
+        <v>0</v>
+      </c>
+      <c r="BC8" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>2060</v>
       </c>
@@ -1378,8 +1487,26 @@
       <c r="AV9" s="5">
         <v>8.8229397874300955E-5</v>
       </c>
+      <c r="AX9" s="5">
+        <v>2060</v>
+      </c>
+      <c r="AY9" s="5">
+        <v>7.1155643087639217E-5</v>
+      </c>
+      <c r="AZ9" s="5">
+        <v>7.2944555823906132E-5</v>
+      </c>
+      <c r="BA9" s="5">
+        <v>7.508513712286557E-5</v>
+      </c>
+      <c r="BB9" s="5">
+        <v>7.6260473212275143E-5</v>
+      </c>
+      <c r="BC9" s="5">
+        <v>8.8229397874300955E-5</v>
+      </c>
     </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>2080</v>
       </c>
@@ -1506,8 +1633,26 @@
       <c r="AV10" s="5">
         <v>1.7364025824845309E-5</v>
       </c>
+      <c r="AX10" s="5">
+        <v>2080</v>
+      </c>
+      <c r="AY10" s="5">
+        <v>1.3418894915573354E-5</v>
+      </c>
+      <c r="AZ10" s="5">
+        <v>1.4055531157619593E-5</v>
+      </c>
+      <c r="BA10" s="5">
+        <v>1.4544777158365107E-5</v>
+      </c>
+      <c r="BB10" s="5">
+        <v>1.4165668575349955E-5</v>
+      </c>
+      <c r="BC10" s="5">
+        <v>1.7364025824845309E-5</v>
+      </c>
     </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>2100</v>
       </c>
@@ -1634,8 +1779,26 @@
       <c r="AV11" s="5">
         <v>7.3930841433478277E-7</v>
       </c>
+      <c r="AX11" s="5">
+        <v>2100</v>
+      </c>
+      <c r="AY11" s="5">
+        <v>5.4923995536082519E-7</v>
+      </c>
+      <c r="AZ11" s="5">
+        <v>5.9687074613901105E-7</v>
+      </c>
+      <c r="BA11" s="5">
+        <v>6.1714408356783323E-7</v>
+      </c>
+      <c r="BB11" s="5">
+        <v>5.7665128834427647E-7</v>
+      </c>
+      <c r="BC11" s="5">
+        <v>7.3930841433478277E-7</v>
+      </c>
     </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>2200</v>
       </c>
@@ -1762,8 +1925,26 @@
       <c r="AV12" s="5">
         <v>1.2292778128752957E-10</v>
       </c>
+      <c r="AX12" s="5">
+        <v>2200</v>
+      </c>
+      <c r="AY12" s="5">
+        <v>9.0322458401459472E-11</v>
+      </c>
+      <c r="AZ12" s="5">
+        <v>9.9343540060914399E-11</v>
+      </c>
+      <c r="BA12" s="5">
+        <v>1.0258888849534743E-10</v>
+      </c>
+      <c r="BB12" s="5">
+        <v>9.4655263627174685E-11</v>
+      </c>
+      <c r="BC12" s="5">
+        <v>1.2292778128752957E-10</v>
+      </c>
     </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>2300</v>
       </c>
@@ -1890,13 +2071,31 @@
       <c r="AV13" s="5">
         <v>1.7053025658242404E-13</v>
       </c>
+      <c r="AX13" s="5">
+        <v>2300</v>
+      </c>
+      <c r="AY13" s="5">
+        <v>1.2501111257279263E-13</v>
+      </c>
+      <c r="AZ13" s="5">
+        <v>1.3788969965844444E-13</v>
+      </c>
+      <c r="BA13" s="5">
+        <v>1.4233059175694507E-13</v>
+      </c>
+      <c r="BB13" s="5">
+        <v>1.3145040611561853E-13</v>
+      </c>
+      <c r="BC13" s="5">
+        <v>1.7053025658242404E-13</v>
+      </c>
     </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -1918,8 +2117,11 @@
       <c r="AQ16" t="s">
         <v>20</v>
       </c>
+      <c r="AX16" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="17" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
@@ -2051,8 +2253,26 @@
       <c r="AV17" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="AX17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="AY17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AZ17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="BA17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="BB17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="BC17" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="18" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>2010</v>
       </c>
@@ -2179,8 +2399,26 @@
       <c r="AV18" s="5">
         <v>0</v>
       </c>
+      <c r="AX18" s="5">
+        <v>2010</v>
+      </c>
+      <c r="AY18" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ18" s="5">
+        <v>0</v>
+      </c>
+      <c r="BA18" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB18" s="5">
+        <v>0</v>
+      </c>
+      <c r="BC18" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>2020</v>
       </c>
@@ -2307,8 +2545,26 @@
       <c r="AV19" s="5">
         <v>0</v>
       </c>
+      <c r="AX19" s="5">
+        <v>2020</v>
+      </c>
+      <c r="AY19" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ19" s="5">
+        <v>0</v>
+      </c>
+      <c r="BA19" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB19" s="5">
+        <v>0</v>
+      </c>
+      <c r="BC19" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>2030</v>
       </c>
@@ -2435,8 +2691,26 @@
       <c r="AV20" s="5">
         <v>0</v>
       </c>
+      <c r="AX20" s="5">
+        <v>2030</v>
+      </c>
+      <c r="AY20" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ20" s="5">
+        <v>0</v>
+      </c>
+      <c r="BA20" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB20" s="5">
+        <v>0</v>
+      </c>
+      <c r="BC20" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>2040</v>
       </c>
@@ -2563,8 +2837,26 @@
       <c r="AV21" s="5">
         <v>0</v>
       </c>
+      <c r="AX21" s="5">
+        <v>2040</v>
+      </c>
+      <c r="AY21" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ21" s="5">
+        <v>0</v>
+      </c>
+      <c r="BA21" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB21" s="5">
+        <v>0</v>
+      </c>
+      <c r="BC21" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>2050</v>
       </c>
@@ -2691,8 +2983,26 @@
       <c r="AV22" s="5">
         <v>0</v>
       </c>
+      <c r="AX22" s="5">
+        <v>2050</v>
+      </c>
+      <c r="AY22" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ22" s="5">
+        <v>0</v>
+      </c>
+      <c r="BA22" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB22" s="5">
+        <v>0</v>
+      </c>
+      <c r="BC22" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>2060</v>
       </c>
@@ -2819,8 +3129,26 @@
       <c r="AV23" s="5">
         <v>3.4154397442547058E-4</v>
       </c>
+      <c r="AX23" s="5">
+        <v>2060</v>
+      </c>
+      <c r="AY23" s="5">
+        <v>3.4756994042368374E-4</v>
+      </c>
+      <c r="AZ23" s="5">
+        <v>3.2965924978970161E-4</v>
+      </c>
+      <c r="BA23" s="5">
+        <v>3.2867020376360357E-4</v>
+      </c>
+      <c r="BB23" s="5">
+        <v>3.3633103433914903E-4</v>
+      </c>
+      <c r="BC23" s="5">
+        <v>3.4154397442547058E-4</v>
+      </c>
     </row>
-    <row r="24" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>2080</v>
       </c>
@@ -2947,8 +3275,26 @@
       <c r="AV24" s="5">
         <v>2.9949878678081908E-4</v>
       </c>
+      <c r="AX24" s="5">
+        <v>2080</v>
+      </c>
+      <c r="AY24" s="5">
+        <v>3.0442179878799878E-4</v>
+      </c>
+      <c r="AZ24" s="5">
+        <v>2.8776869401197781E-4</v>
+      </c>
+      <c r="BA24" s="5">
+        <v>2.8413111429783646E-4</v>
+      </c>
+      <c r="BB24" s="5">
+        <v>2.9299055979585542E-4</v>
+      </c>
+      <c r="BC24" s="5">
+        <v>2.9949878678081908E-4</v>
+      </c>
     </row>
-    <row r="25" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>2100</v>
       </c>
@@ -3075,8 +3421,26 @@
       <c r="AV25" s="5">
         <v>1.7937031897590828E-4</v>
       </c>
+      <c r="AX25" s="5">
+        <v>2100</v>
+      </c>
+      <c r="AY25" s="5">
+        <v>1.8109292692546631E-4</v>
+      </c>
+      <c r="AZ25" s="5">
+        <v>1.7303499667413347E-4</v>
+      </c>
+      <c r="BA25" s="5">
+        <v>1.6545806484028424E-4</v>
+      </c>
+      <c r="BB25" s="5">
+        <v>1.7257920543678807E-4</v>
+      </c>
+      <c r="BC25" s="5">
+        <v>1.7937031897590828E-4</v>
+      </c>
     </row>
-    <row r="26" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>2200</v>
       </c>
@@ -3203,8 +3567,26 @@
       <c r="AV26" s="5">
         <v>7.3215175532643782E-5</v>
       </c>
+      <c r="AX26" s="5">
+        <v>2200</v>
+      </c>
+      <c r="AY26" s="5">
+        <v>7.3388024830025605E-5</v>
+      </c>
+      <c r="AZ26" s="5">
+        <v>7.101522016244311E-5</v>
+      </c>
+      <c r="BA26" s="5">
+        <v>6.5696502927544692E-5</v>
+      </c>
+      <c r="BB26" s="5">
+        <v>6.9260370142663059E-5</v>
+      </c>
+      <c r="BC26" s="5">
+        <v>7.3215175532643782E-5</v>
+      </c>
     </row>
-    <row r="27" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>2300</v>
       </c>
@@ -3329,6 +3711,24 @@
         <v>4.2597198992688767E-5</v>
       </c>
       <c r="AV27" s="5">
+        <v>4.5240913177369002E-5</v>
+      </c>
+      <c r="AX27" s="5">
+        <v>2300</v>
+      </c>
+      <c r="AY27" s="5">
+        <v>4.5256296990203726E-5</v>
+      </c>
+      <c r="AZ27" s="5">
+        <v>4.3949774506890638E-5</v>
+      </c>
+      <c r="BA27" s="5">
+        <v>4.0290512913099263E-5</v>
+      </c>
+      <c r="BB27" s="5">
+        <v>4.2597198992688767E-5</v>
+      </c>
+      <c r="BC27" s="5">
         <v>4.5240913177369002E-5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add perturbations for CH4 and N2O out to 2080
</commit_message>
<xml_diff>
--- a/data/IWG_inputs/PAGE/Non-co2 perturbation data - 1 Mt.xlsx
+++ b/data/IWG_inputs/PAGE/Non-co2 perturbation data - 1 Mt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bparthum\.julia\dev\MimiIWG\data\IWG_inputs\PAGE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B500360-86E1-415D-A492-0F8D2E619F2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A71D2A-7CE4-4D23-8218-6268B7E508C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="23">
   <si>
     <t>Pertubation in the PAGE Excess Forcings vector due to a 1 Mt shock in CH4</t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t>PAGE input: N2O Shock, 2060</t>
+  </si>
+  <si>
+    <t>PAGE input: CH4 Shock, 2080</t>
+  </si>
+  <si>
+    <t>PAGE input: N2O Shock, 2080</t>
   </si>
 </sst>
 </file>
@@ -442,20 +448,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AV27"/>
+  <dimension ref="A1:BC27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AR4" sqref="AR4"/>
+    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
+      <selection activeCell="AZ14" sqref="AZ14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -477,8 +483,11 @@
       <c r="AQ2" t="s">
         <v>19</v>
       </c>
+      <c r="AX2" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -610,8 +619,26 @@
       <c r="AV3" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="AX3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="AY3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AZ3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="BA3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="BB3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="BC3" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2010</v>
       </c>
@@ -738,8 +765,26 @@
       <c r="AV4" s="5">
         <v>0</v>
       </c>
+      <c r="AX4" s="5">
+        <v>2010</v>
+      </c>
+      <c r="AY4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ4" s="5">
+        <v>0</v>
+      </c>
+      <c r="BA4" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB4" s="5">
+        <v>0</v>
+      </c>
+      <c r="BC4" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2020</v>
       </c>
@@ -866,8 +911,26 @@
       <c r="AV5" s="5">
         <v>0</v>
       </c>
+      <c r="AX5" s="5">
+        <v>2020</v>
+      </c>
+      <c r="AY5" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ5" s="5">
+        <v>0</v>
+      </c>
+      <c r="BA5" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB5" s="5">
+        <v>0</v>
+      </c>
+      <c r="BC5" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>2030</v>
       </c>
@@ -994,8 +1057,26 @@
       <c r="AV6" s="5">
         <v>0</v>
       </c>
+      <c r="AX6" s="5">
+        <v>2030</v>
+      </c>
+      <c r="AY6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ6" s="5">
+        <v>0</v>
+      </c>
+      <c r="BA6" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB6" s="5">
+        <v>0</v>
+      </c>
+      <c r="BC6" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>2040</v>
       </c>
@@ -1122,8 +1203,26 @@
       <c r="AV7" s="5">
         <v>0</v>
       </c>
+      <c r="AX7" s="5">
+        <v>2040</v>
+      </c>
+      <c r="AY7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ7" s="5">
+        <v>0</v>
+      </c>
+      <c r="BA7" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB7" s="5">
+        <v>0</v>
+      </c>
+      <c r="BC7" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>2050</v>
       </c>
@@ -1250,8 +1349,26 @@
       <c r="AV8" s="5">
         <v>0</v>
       </c>
+      <c r="AX8" s="5">
+        <v>2050</v>
+      </c>
+      <c r="AY8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ8" s="5">
+        <v>0</v>
+      </c>
+      <c r="BA8" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB8" s="5">
+        <v>0</v>
+      </c>
+      <c r="BC8" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>2060</v>
       </c>
@@ -1378,8 +1495,26 @@
       <c r="AV9" s="5">
         <v>8.8229397874300955E-5</v>
       </c>
+      <c r="AX9" s="5">
+        <v>2060</v>
+      </c>
+      <c r="AY9" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ9" s="5">
+        <v>0</v>
+      </c>
+      <c r="BA9" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB9" s="5">
+        <v>0</v>
+      </c>
+      <c r="BC9" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>2080</v>
       </c>
@@ -1506,8 +1641,26 @@
       <c r="AV10" s="5">
         <v>1.7364025824845309E-5</v>
       </c>
+      <c r="AX10" s="5">
+        <v>2080</v>
+      </c>
+      <c r="AY10" s="5">
+        <v>7.2240264871450524E-5</v>
+      </c>
+      <c r="AZ10" s="5">
+        <v>7.5769316062878004E-5</v>
+      </c>
+      <c r="BA10" s="5">
+        <v>7.8418998831559543E-5</v>
+      </c>
+      <c r="BB10" s="5">
+        <v>7.6237339676625473E-5</v>
+      </c>
+      <c r="BC10" s="5">
+        <v>9.3649217227735539E-5</v>
+      </c>
     </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>2100</v>
       </c>
@@ -1634,8 +1787,26 @@
       <c r="AV11" s="5">
         <v>7.3930841433478277E-7</v>
       </c>
+      <c r="AX11" s="5">
+        <v>2100</v>
+      </c>
+      <c r="AY11" s="5">
+        <v>3.1299133349849127E-6</v>
+      </c>
+      <c r="AZ11" s="5">
+        <v>3.4013421684231383E-6</v>
+      </c>
+      <c r="BA11" s="5">
+        <v>3.5168716620059827E-6</v>
+      </c>
+      <c r="BB11" s="5">
+        <v>3.2861195249855866E-6</v>
+      </c>
+      <c r="BC11" s="5">
+        <v>4.2130350609481668E-6</v>
+      </c>
     </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>2200</v>
       </c>
@@ -1762,8 +1933,26 @@
       <c r="AV12" s="5">
         <v>1.2292778128752957E-10</v>
       </c>
+      <c r="AX12" s="5">
+        <v>2200</v>
+      </c>
+      <c r="AY12" s="5">
+        <v>5.1471513939915784E-10</v>
+      </c>
+      <c r="AZ12" s="5">
+        <v>5.6612308174663899E-10</v>
+      </c>
+      <c r="BA12" s="5">
+        <v>5.8461658847264171E-10</v>
+      </c>
+      <c r="BB12" s="5">
+        <v>5.3940619304526645E-10</v>
+      </c>
+      <c r="BC12" s="5">
+        <v>7.00520939034277E-10</v>
+      </c>
     </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>2300</v>
       </c>
@@ -1890,13 +2079,31 @@
       <c r="AV13" s="5">
         <v>1.7053025658242404E-13</v>
       </c>
+      <c r="AX13" s="5">
+        <v>2300</v>
+      </c>
+      <c r="AY13" s="5">
+        <v>7.1409544943890069E-13</v>
+      </c>
+      <c r="AZ13" s="5">
+        <v>7.8492767840998567E-13</v>
+      </c>
+      <c r="BA13" s="5">
+        <v>8.1090689718621434E-13</v>
+      </c>
+      <c r="BB13" s="5">
+        <v>7.4784622938750545E-13</v>
+      </c>
+      <c r="BC13" s="5">
+        <v>9.7144514654701197E-13</v>
+      </c>
     </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -1918,8 +2125,11 @@
       <c r="AQ16" t="s">
         <v>20</v>
       </c>
+      <c r="AX16" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="17" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
@@ -2051,8 +2261,26 @@
       <c r="AV17" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="AX17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="AY17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AZ17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="BA17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="BB17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="BC17" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="18" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>2010</v>
       </c>
@@ -2179,8 +2407,26 @@
       <c r="AV18" s="5">
         <v>0</v>
       </c>
+      <c r="AX18" s="5">
+        <v>2010</v>
+      </c>
+      <c r="AY18" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ18" s="5">
+        <v>0</v>
+      </c>
+      <c r="BA18" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB18" s="5">
+        <v>0</v>
+      </c>
+      <c r="BC18" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>2020</v>
       </c>
@@ -2307,8 +2553,26 @@
       <c r="AV19" s="5">
         <v>0</v>
       </c>
+      <c r="AX19" s="5">
+        <v>2020</v>
+      </c>
+      <c r="AY19" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ19" s="5">
+        <v>0</v>
+      </c>
+      <c r="BA19" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB19" s="5">
+        <v>0</v>
+      </c>
+      <c r="BC19" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>2030</v>
       </c>
@@ -2435,8 +2699,26 @@
       <c r="AV20" s="5">
         <v>0</v>
       </c>
+      <c r="AX20" s="5">
+        <v>2030</v>
+      </c>
+      <c r="AY20" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ20" s="5">
+        <v>0</v>
+      </c>
+      <c r="BA20" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB20" s="5">
+        <v>0</v>
+      </c>
+      <c r="BC20" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>2040</v>
       </c>
@@ -2563,8 +2845,26 @@
       <c r="AV21" s="5">
         <v>0</v>
       </c>
+      <c r="AX21" s="5">
+        <v>2040</v>
+      </c>
+      <c r="AY21" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ21" s="5">
+        <v>0</v>
+      </c>
+      <c r="BA21" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB21" s="5">
+        <v>0</v>
+      </c>
+      <c r="BC21" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>2050</v>
       </c>
@@ -2691,8 +2991,26 @@
       <c r="AV22" s="5">
         <v>0</v>
       </c>
+      <c r="AX22" s="5">
+        <v>2050</v>
+      </c>
+      <c r="AY22" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ22" s="5">
+        <v>0</v>
+      </c>
+      <c r="BA22" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB22" s="5">
+        <v>0</v>
+      </c>
+      <c r="BC22" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>2060</v>
       </c>
@@ -2819,8 +3137,26 @@
       <c r="AV23" s="5">
         <v>3.4154397442547058E-4</v>
       </c>
+      <c r="AX23" s="5">
+        <v>2060</v>
+      </c>
+      <c r="AY23" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ23" s="5">
+        <v>0</v>
+      </c>
+      <c r="BA23" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB23" s="5">
+        <v>0</v>
+      </c>
+      <c r="BC23" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="24" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>2080</v>
       </c>
@@ -2947,8 +3283,26 @@
       <c r="AV24" s="5">
         <v>2.9949878678081908E-4</v>
       </c>
+      <c r="AX24" s="5">
+        <v>2080</v>
+      </c>
+      <c r="AY24" s="5">
+        <v>3.6132447295342409E-4</v>
+      </c>
+      <c r="AZ24" s="5">
+        <v>3.415610660511957E-4</v>
+      </c>
+      <c r="BA24" s="5">
+        <v>3.371325169616462E-4</v>
+      </c>
+      <c r="BB24" s="5">
+        <v>3.4770880718886757E-4</v>
+      </c>
+      <c r="BC24" s="5">
+        <v>3.5550284434211548E-4</v>
+      </c>
     </row>
-    <row r="25" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>2100</v>
       </c>
@@ -3075,8 +3429,26 @@
       <c r="AV25" s="5">
         <v>1.7937031897590828E-4</v>
       </c>
+      <c r="AX25" s="5">
+        <v>2100</v>
+      </c>
+      <c r="AY25" s="5">
+        <v>2.1598616098579383E-4</v>
+      </c>
+      <c r="AZ25" s="5">
+        <v>2.0637577727042057E-4</v>
+      </c>
+      <c r="BA25" s="5">
+        <v>1.9733902078532316E-4</v>
+      </c>
+      <c r="BB25" s="5">
+        <v>2.0583216002156179E-4</v>
+      </c>
+      <c r="BC25" s="5">
+        <v>2.1393167721237949E-4</v>
+      </c>
     </row>
-    <row r="26" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>2200</v>
       </c>
@@ -3203,8 +3575,26 @@
       <c r="AV26" s="5">
         <v>7.3215175532643782E-5</v>
       </c>
+      <c r="AX26" s="5">
+        <v>2200</v>
+      </c>
+      <c r="AY26" s="5">
+        <v>8.752898405308795E-5</v>
+      </c>
+      <c r="AZ26" s="5">
+        <v>8.4698988014204611E-5</v>
+      </c>
+      <c r="BA26" s="5">
+        <v>7.8355453610929883E-5</v>
+      </c>
+      <c r="BB26" s="5">
+        <v>8.2606011835180122E-5</v>
+      </c>
+      <c r="BC26" s="5">
+        <v>8.7322830481476044E-5</v>
+      </c>
     </row>
-    <row r="27" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>2300</v>
       </c>
@@ -3330,6 +3720,24 @@
       </c>
       <c r="AV27" s="5">
         <v>4.5240913177369002E-5</v>
+      </c>
+      <c r="AX27" s="5">
+        <v>2300</v>
+      </c>
+      <c r="AY27" s="5">
+        <v>5.3976699967039909E-5</v>
+      </c>
+      <c r="AZ27" s="5">
+        <v>5.241843039205385E-5</v>
+      </c>
+      <c r="BA27" s="5">
+        <v>4.8054081898007972E-5</v>
+      </c>
+      <c r="BB27" s="5">
+        <v>5.0805233537953853E-5</v>
+      </c>
+      <c r="BC27" s="5">
+        <v>5.3958351930005755E-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>